<commit_message>
Working on displaying New Student Info to Gui screen.
</commit_message>
<xml_diff>
--- a/Tkinter/clocking.xlsx
+++ b/Tkinter/clocking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>Freddy Velez</t>
   </si>
@@ -125,6 +125,45 @@
   </si>
   <si>
     <t>IN -&gt; 2017/03/20 12:56</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/20 13:09</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 13:11</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/20 13:11</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 15:57</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/20 20:56</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 20:56</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/20 20:57</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 20:58</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/20 21:43</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 21:43</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/20 22:50</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 22:50</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/20 23:04</t>
   </si>
 </sst>
 </file>
@@ -493,7 +532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
@@ -728,6 +767,86 @@
         <v>36</v>
       </c>
     </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>

<commit_message>
Made some profress on new student function. Still haven't resolved issue
</commit_message>
<xml_diff>
--- a/Tkinter/clocking.xlsx
+++ b/Tkinter/clocking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Freddy Velez</t>
   </si>
@@ -164,6 +164,72 @@
   </si>
   <si>
     <t>IN -&gt; 2017/03/20 23:04</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/23 15:49</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/23 15:50</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/23 15:52</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/23 15:53</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/23 15:53</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/23 15:55</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 14:55</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 14:57</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:02</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:02</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:04</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:05</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:07</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:08</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:11</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:11</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:14</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:15</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:16</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:17</t>
+  </si>
+  <si>
+    <t>OUT -&gt; 2017/03/27 15:22</t>
+  </si>
+  <si>
+    <t>IN -&gt; 2017/03/27 15:25</t>
   </si>
 </sst>
 </file>
@@ -532,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
@@ -847,6 +913,116 @@
         <v>49</v>
       </c>
     </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>